<commit_message>
Analysis of Oct 2021
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR26"/>
+  <dimension ref="A1:CG26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,6 +653,211 @@
           <t>Additional specifications 3</t>
         </is>
       </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Date of + test</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Symptoms prior to admit</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Fever</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>SOB</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Cough</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Sinus Congestion</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Malaise or Fatigue or Weakness</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Diarrhea</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Confusion</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Anorexia</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Myalgias Athralgias</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>HA</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Sore throat</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Abdominal pain</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>SIRS criteria met on admission</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>Temp</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>SBP</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>DBP</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>Pulse</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>RR</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>O2</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>WBC</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>SIRS criteria met</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>Supp O2</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>MI</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>CHF</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>PVD</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>CVA or TIA</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>Dementia</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>COPD</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>Connective tissue disease</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>PUD</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>Liver disease</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>Mod-Sev CKD</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>Solid tumor</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>Leukemia</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>Lymphoma</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>AIDS</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>Hemiplegia</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>Days after admit test positive</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -827,6 +1032,173 @@
       <c r="AP2" t="inlineStr"/>
       <c r="AQ2" t="inlineStr"/>
       <c r="AR2" t="inlineStr"/>
+      <c r="AS2" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BH2" t="n">
+        <v>102</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>107</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>59</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>70</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>21</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>7.79</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>5</v>
+      </c>
+      <c r="BQ2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BW2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BX2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr">
+        <is>
+          <t>Yes/Complicated</t>
+        </is>
+      </c>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC2" t="inlineStr"/>
+      <c r="CD2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1011,6 +1383,173 @@
       <c r="AP3" t="inlineStr"/>
       <c r="AQ3" t="inlineStr"/>
       <c r="AR3" t="inlineStr"/>
+      <c r="AS3" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH3" t="n">
+        <v>98</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>145</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>70</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>70</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY3" t="inlineStr"/>
+      <c r="BZ3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA3" t="inlineStr"/>
+      <c r="CB3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CC3" t="inlineStr"/>
+      <c r="CD3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE3" t="inlineStr"/>
+      <c r="CF3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1185,6 +1724,173 @@
       <c r="AP4" t="inlineStr"/>
       <c r="AQ4" t="inlineStr"/>
       <c r="AR4" t="inlineStr"/>
+      <c r="AS4" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="AT4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BD4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH4" t="n">
+        <v>99.5</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>132</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>65</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>90</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>4.46</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BQ4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BW4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1357,6 +2063,173 @@
       <c r="AP5" t="inlineStr"/>
       <c r="AQ5" t="inlineStr"/>
       <c r="AR5" t="inlineStr"/>
+      <c r="AS5" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH5" t="n">
+        <v>97.8</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>92</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>64</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>62</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>17</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>11.02</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BT5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY5" t="inlineStr"/>
+      <c r="BZ5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA5" t="inlineStr"/>
+      <c r="CB5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC5" t="inlineStr"/>
+      <c r="CD5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE5" t="inlineStr"/>
+      <c r="CF5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1529,6 +2402,173 @@
       <c r="AP6" t="inlineStr"/>
       <c r="AQ6" t="inlineStr"/>
       <c r="AR6" t="inlineStr"/>
+      <c r="AS6" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH6" t="n">
+        <v>100</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>144</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>65</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>78</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>22</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>6.32</v>
+      </c>
+      <c r="BO6" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP6" t="n">
+        <v>2</v>
+      </c>
+      <c r="BQ6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY6" t="inlineStr"/>
+      <c r="BZ6" t="inlineStr">
+        <is>
+          <t>Yes/Uncomplicated</t>
+        </is>
+      </c>
+      <c r="CA6" t="inlineStr"/>
+      <c r="CB6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC6" t="inlineStr"/>
+      <c r="CD6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE6" t="inlineStr"/>
+      <c r="CF6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1701,6 +2741,173 @@
       <c r="AP7" t="inlineStr"/>
       <c r="AQ7" t="inlineStr"/>
       <c r="AR7" t="inlineStr"/>
+      <c r="AS7" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="AT7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH7" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>121</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>72</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>86</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY7" t="inlineStr"/>
+      <c r="BZ7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA7" t="inlineStr"/>
+      <c r="CB7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC7" t="inlineStr"/>
+      <c r="CD7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE7" t="inlineStr"/>
+      <c r="CF7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1869,6 +3076,173 @@
       <c r="AP8" t="inlineStr"/>
       <c r="AQ8" t="inlineStr"/>
       <c r="AR8" t="inlineStr"/>
+      <c r="AS8" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="AT8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BH8" t="n">
+        <v>100.5</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>174</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>73</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>62</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>24</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>6.08</v>
+      </c>
+      <c r="BO8" t="n">
+        <v>2</v>
+      </c>
+      <c r="BP8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY8" t="inlineStr"/>
+      <c r="BZ8" t="inlineStr">
+        <is>
+          <t>Yes/Complicated</t>
+        </is>
+      </c>
+      <c r="CA8" t="inlineStr"/>
+      <c r="CB8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC8" t="inlineStr"/>
+      <c r="CD8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE8" t="inlineStr"/>
+      <c r="CF8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG8" t="n">
+        <v>-1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1942,7 +3316,11 @@
       <c r="Q9" s="2" t="n">
         <v>39919</v>
       </c>
-      <c r="R9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
       <c r="S9" t="inlineStr">
         <is>
           <t>No</t>
@@ -2035,6 +3413,173 @@
       <c r="AP9" t="inlineStr"/>
       <c r="AQ9" t="inlineStr"/>
       <c r="AR9" t="inlineStr"/>
+      <c r="AS9" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="AT9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AU9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH9" t="n">
+        <v>98.3</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>150</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>66</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>86</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>7.74</v>
+      </c>
+      <c r="BO9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY9" t="inlineStr"/>
+      <c r="BZ9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA9" t="inlineStr"/>
+      <c r="CB9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC9" t="inlineStr"/>
+      <c r="CD9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE9" t="inlineStr"/>
+      <c r="CF9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -2203,6 +3748,173 @@
       <c r="AP10" t="inlineStr"/>
       <c r="AQ10" t="inlineStr"/>
       <c r="AR10" t="inlineStr"/>
+      <c r="AS10" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="AT10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AU10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BC10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH10" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>146</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>67</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>75</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>29</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="BN10" t="n">
+        <v>9.859999999999999</v>
+      </c>
+      <c r="BO10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY10" t="inlineStr"/>
+      <c r="BZ10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA10" t="inlineStr"/>
+      <c r="CB10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC10" t="inlineStr"/>
+      <c r="CD10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE10" t="inlineStr"/>
+      <c r="CF10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -2377,6 +4089,173 @@
       <c r="AP11" t="inlineStr"/>
       <c r="AQ11" t="inlineStr"/>
       <c r="AR11" t="inlineStr"/>
+      <c r="AS11" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="AT11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AY11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BC11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BH11" t="n">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>141</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>81</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>101</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>24</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="BN11" t="n">
+        <v>7.71</v>
+      </c>
+      <c r="BO11" t="n">
+        <v>2</v>
+      </c>
+      <c r="BP11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY11" t="inlineStr"/>
+      <c r="BZ11" t="inlineStr">
+        <is>
+          <t>Yes/Complicated</t>
+        </is>
+      </c>
+      <c r="CA11" t="inlineStr"/>
+      <c r="CB11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC11" t="inlineStr"/>
+      <c r="CD11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE11" t="inlineStr"/>
+      <c r="CF11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -2543,6 +4422,171 @@
       <c r="AP12" t="inlineStr"/>
       <c r="AQ12" t="inlineStr"/>
       <c r="AR12" t="inlineStr"/>
+      <c r="AS12" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="AT12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BC12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BE12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH12" t="n">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>90</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>60</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>72</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="BN12" t="inlineStr"/>
+      <c r="BO12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY12" t="inlineStr"/>
+      <c r="BZ12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA12" t="inlineStr"/>
+      <c r="CB12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC12" t="inlineStr"/>
+      <c r="CD12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE12" t="inlineStr"/>
+      <c r="CF12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -2616,7 +4660,11 @@
       <c r="Q13" s="2" t="n">
         <v>41226</v>
       </c>
-      <c r="R13" t="inlineStr"/>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
       <c r="S13" t="inlineStr">
         <is>
           <t>No</t>
@@ -2721,6 +4769,173 @@
       <c r="AP13" t="inlineStr"/>
       <c r="AQ13" t="inlineStr"/>
       <c r="AR13" t="inlineStr"/>
+      <c r="AS13" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="AT13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH13" t="n">
+        <v>99.2</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>161</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>82</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>89</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>24</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="BN13" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="BO13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP13" t="n">
+        <v>2</v>
+      </c>
+      <c r="BQ13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY13" t="inlineStr"/>
+      <c r="BZ13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA13" t="inlineStr"/>
+      <c r="CB13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC13" t="inlineStr"/>
+      <c r="CD13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE13" t="inlineStr"/>
+      <c r="CF13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CG13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -2895,6 +5110,173 @@
       <c r="AP14" t="inlineStr"/>
       <c r="AQ14" t="inlineStr"/>
       <c r="AR14" t="inlineStr"/>
+      <c r="AS14" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="AT14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH14" t="n">
+        <v>98.59999999999999</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>128</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>62</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>76</v>
+      </c>
+      <c r="BL14" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM14" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="BN14" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="BO14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BY14" t="inlineStr"/>
+      <c r="BZ14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA14" t="inlineStr"/>
+      <c r="CB14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC14" t="inlineStr"/>
+      <c r="CD14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE14" t="inlineStr"/>
+      <c r="CF14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -3063,6 +5445,173 @@
       <c r="AP15" t="inlineStr"/>
       <c r="AQ15" t="inlineStr"/>
       <c r="AR15" t="inlineStr"/>
+      <c r="AS15" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="AT15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AU15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH15" t="n">
+        <v>98.3</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>90</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>58</v>
+      </c>
+      <c r="BK15" t="n">
+        <v>70</v>
+      </c>
+      <c r="BL15" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM15" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="BN15" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="BO15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY15" t="inlineStr"/>
+      <c r="BZ15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA15" t="inlineStr"/>
+      <c r="CB15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC15" t="inlineStr"/>
+      <c r="CD15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE15" t="inlineStr"/>
+      <c r="CF15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CG15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -3138,7 +5687,11 @@
           <t>Unknown</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr"/>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>DNR/DNI</t>
+        </is>
+      </c>
       <c r="S16" t="inlineStr">
         <is>
           <t>No</t>
@@ -3235,6 +5788,173 @@
       <c r="AP16" t="inlineStr"/>
       <c r="AQ16" t="inlineStr"/>
       <c r="AR16" t="inlineStr"/>
+      <c r="AS16" s="2" t="n">
+        <v>44346</v>
+      </c>
+      <c r="AT16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AU16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH16" t="n">
+        <v>98.7</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>143</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>99</v>
+      </c>
+      <c r="BK16" t="n">
+        <v>81</v>
+      </c>
+      <c r="BL16" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM16" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="BN16" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="BO16" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BY16" t="inlineStr"/>
+      <c r="BZ16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA16" t="inlineStr"/>
+      <c r="CB16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CC16" t="inlineStr"/>
+      <c r="CD16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE16" t="inlineStr"/>
+      <c r="CF16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG16" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -3421,6 +6141,173 @@
       <c r="AP17" t="inlineStr"/>
       <c r="AQ17" t="inlineStr"/>
       <c r="AR17" t="inlineStr"/>
+      <c r="AS17" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="AT17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BE17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BH17" t="n">
+        <v>100.6</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>111</v>
+      </c>
+      <c r="BJ17" t="n">
+        <v>69</v>
+      </c>
+      <c r="BK17" t="n">
+        <v>120</v>
+      </c>
+      <c r="BL17" t="n">
+        <v>22</v>
+      </c>
+      <c r="BM17" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BN17" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="BO17" t="n">
+        <v>4</v>
+      </c>
+      <c r="BP17" t="n">
+        <v>4</v>
+      </c>
+      <c r="BQ17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BW17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BY17" t="inlineStr"/>
+      <c r="BZ17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA17" t="inlineStr"/>
+      <c r="CB17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CC17" t="inlineStr"/>
+      <c r="CD17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="CE17" t="inlineStr"/>
+      <c r="CF17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -3595,6 +6482,173 @@
       <c r="AP18" t="inlineStr"/>
       <c r="AQ18" t="inlineStr"/>
       <c r="AR18" t="inlineStr"/>
+      <c r="AS18" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="AT18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH18" t="n">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>144</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>70</v>
+      </c>
+      <c r="BK18" t="n">
+        <v>71</v>
+      </c>
+      <c r="BL18" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM18" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BN18" t="n">
+        <v>7.85</v>
+      </c>
+      <c r="BO18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP18" t="n">
+        <v>2</v>
+      </c>
+      <c r="BQ18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY18" t="inlineStr"/>
+      <c r="BZ18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA18" t="inlineStr"/>
+      <c r="CB18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC18" t="inlineStr"/>
+      <c r="CD18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE18" t="inlineStr"/>
+      <c r="CF18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -3763,6 +6817,173 @@
       <c r="AP19" t="inlineStr"/>
       <c r="AQ19" t="inlineStr"/>
       <c r="AR19" t="inlineStr"/>
+      <c r="AS19" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="AT19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BF19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BG19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH19" t="n">
+        <v>97.7</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>100</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>74</v>
+      </c>
+      <c r="BK19" t="n">
+        <v>114</v>
+      </c>
+      <c r="BL19" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM19" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="BN19" t="n">
+        <v>7.91</v>
+      </c>
+      <c r="BO19" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY19" t="inlineStr"/>
+      <c r="BZ19" t="inlineStr">
+        <is>
+          <t>Yes/Complicated</t>
+        </is>
+      </c>
+      <c r="CA19" t="inlineStr"/>
+      <c r="CB19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC19" t="inlineStr"/>
+      <c r="CD19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE19" t="inlineStr"/>
+      <c r="CF19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG19" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -3836,7 +7057,11 @@
       <c r="Q20" s="2" t="n">
         <v>43447</v>
       </c>
-      <c r="R20" t="inlineStr"/>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Full code</t>
+        </is>
+      </c>
       <c r="S20" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -3927,6 +7152,173 @@
       <c r="AP20" t="inlineStr"/>
       <c r="AQ20" t="inlineStr"/>
       <c r="AR20" t="inlineStr"/>
+      <c r="AS20" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="AT20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH20" t="n">
+        <v>97.90000000000001</v>
+      </c>
+      <c r="BI20" t="n">
+        <v>146</v>
+      </c>
+      <c r="BJ20" t="n">
+        <v>71</v>
+      </c>
+      <c r="BK20" t="n">
+        <v>78</v>
+      </c>
+      <c r="BL20" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM20" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="BN20" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="BO20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY20" t="inlineStr"/>
+      <c r="BZ20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA20" t="inlineStr"/>
+      <c r="CB20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC20" t="inlineStr"/>
+      <c r="CD20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE20" t="inlineStr"/>
+      <c r="CF20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -4000,7 +7392,11 @@
       <c r="Q21" t="n">
         <v>2017</v>
       </c>
-      <c r="R21" t="inlineStr"/>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>DNR/DNI</t>
+        </is>
+      </c>
       <c r="S21" t="inlineStr">
         <is>
           <t>No</t>
@@ -4097,6 +7493,173 @@
       <c r="AP21" t="inlineStr"/>
       <c r="AQ21" t="inlineStr"/>
       <c r="AR21" t="inlineStr"/>
+      <c r="AS21" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="AT21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BH21" t="n">
+        <v>98.2</v>
+      </c>
+      <c r="BI21" t="n">
+        <v>143</v>
+      </c>
+      <c r="BJ21" t="n">
+        <v>93</v>
+      </c>
+      <c r="BK21" t="n">
+        <v>102</v>
+      </c>
+      <c r="BL21" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM21" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BN21" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="BO21" t="n">
+        <v>2</v>
+      </c>
+      <c r="BP21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY21" t="inlineStr"/>
+      <c r="BZ21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA21" t="inlineStr"/>
+      <c r="CB21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC21" t="inlineStr"/>
+      <c r="CD21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE21" t="inlineStr"/>
+      <c r="CF21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -4271,6 +7834,173 @@
       <c r="AP22" t="inlineStr"/>
       <c r="AQ22" t="inlineStr"/>
       <c r="AR22" t="inlineStr"/>
+      <c r="AS22" s="2" t="n">
+        <v>44344</v>
+      </c>
+      <c r="AT22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AV22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BC22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH22" t="n">
+        <v>98.59999999999999</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>112</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>69</v>
+      </c>
+      <c r="BK22" t="n">
+        <v>73</v>
+      </c>
+      <c r="BL22" t="n">
+        <v>16</v>
+      </c>
+      <c r="BM22" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="BN22" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="BO22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP22" t="n">
+        <v>2</v>
+      </c>
+      <c r="BQ22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY22" t="inlineStr"/>
+      <c r="BZ22" t="inlineStr">
+        <is>
+          <t>Yes/Complicated</t>
+        </is>
+      </c>
+      <c r="CA22" t="inlineStr"/>
+      <c r="CB22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC22" t="inlineStr"/>
+      <c r="CD22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE22" t="inlineStr"/>
+      <c r="CF22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG22" t="n">
+        <v>-7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -4344,7 +8074,11 @@
       <c r="Q23" s="2" t="n">
         <v>42649</v>
       </c>
-      <c r="R23" t="inlineStr"/>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
       <c r="S23" t="inlineStr">
         <is>
           <t>No</t>
@@ -4437,6 +8171,173 @@
       <c r="AP23" t="inlineStr"/>
       <c r="AQ23" t="inlineStr"/>
       <c r="AR23" t="inlineStr"/>
+      <c r="AS23" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="AT23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AU23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH23" t="n">
+        <v>100.9</v>
+      </c>
+      <c r="BI23" t="n">
+        <v>166</v>
+      </c>
+      <c r="BJ23" t="n">
+        <v>94</v>
+      </c>
+      <c r="BK23" t="n">
+        <v>81</v>
+      </c>
+      <c r="BL23" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM23" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="BN23" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="BO23" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY23" t="inlineStr"/>
+      <c r="BZ23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA23" t="inlineStr"/>
+      <c r="CB23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC23" t="inlineStr"/>
+      <c r="CD23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE23" t="inlineStr"/>
+      <c r="CF23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -4605,6 +8506,173 @@
       <c r="AP24" t="inlineStr"/>
       <c r="AQ24" t="inlineStr"/>
       <c r="AR24" t="inlineStr"/>
+      <c r="AS24" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="AT24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BB24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH24" t="n">
+        <v>98.8</v>
+      </c>
+      <c r="BI24" t="n">
+        <v>113</v>
+      </c>
+      <c r="BJ24" t="n">
+        <v>56</v>
+      </c>
+      <c r="BK24" t="n">
+        <v>71</v>
+      </c>
+      <c r="BL24" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM24" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="BN24" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="BO24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BS24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BV24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY24" t="inlineStr"/>
+      <c r="BZ24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA24" t="inlineStr"/>
+      <c r="CB24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC24" t="inlineStr"/>
+      <c r="CD24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE24" t="inlineStr"/>
+      <c r="CF24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -4807,6 +8875,173 @@
           <t>Comfort</t>
         </is>
       </c>
+      <c r="AS25" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="AT25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AW25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AX25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AZ25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BA25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BH25" t="n">
+        <v>101.1</v>
+      </c>
+      <c r="BI25" t="n">
+        <v>140</v>
+      </c>
+      <c r="BJ25" t="n">
+        <v>69</v>
+      </c>
+      <c r="BK25" t="n">
+        <v>70</v>
+      </c>
+      <c r="BL25" t="n">
+        <v>22</v>
+      </c>
+      <c r="BM25" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="BN25" t="n">
+        <v>11.71</v>
+      </c>
+      <c r="BO25" t="n">
+        <v>2</v>
+      </c>
+      <c r="BP25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BR25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BU25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BW25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY25" t="inlineStr"/>
+      <c r="BZ25" t="inlineStr">
+        <is>
+          <t>Yes/Uncomplicated</t>
+        </is>
+      </c>
+      <c r="CA25" t="inlineStr"/>
+      <c r="CB25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC25" t="inlineStr"/>
+      <c r="CD25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE25" t="inlineStr"/>
+      <c r="CF25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -5006,6 +9241,173 @@
         <is>
           <t>Comfort</t>
         </is>
+      </c>
+      <c r="AS26" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="AT26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AU26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AV26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AX26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="AY26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AZ26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BA26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BB26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BC26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BD26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BE26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BF26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BG26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BH26" t="n">
+        <v>97.7</v>
+      </c>
+      <c r="BI26" t="n">
+        <v>130</v>
+      </c>
+      <c r="BJ26" t="n">
+        <v>68</v>
+      </c>
+      <c r="BK26" t="n">
+        <v>60</v>
+      </c>
+      <c r="BL26" t="n">
+        <v>19</v>
+      </c>
+      <c r="BM26" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="BN26" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="BO26" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BR26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BS26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BT26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BU26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BV26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="BW26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BX26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BY26" t="inlineStr"/>
+      <c r="BZ26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CA26" t="inlineStr"/>
+      <c r="CB26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CC26" t="inlineStr"/>
+      <c r="CD26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CE26" t="inlineStr"/>
+      <c r="CF26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CG26" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>